<commit_message>
Iteration5: Adding built code
</commit_message>
<xml_diff>
--- a/Iteration5/Documents/defect_log-Iteration4.xlsx
+++ b/Iteration5/Documents/defect_log-Iteration4.xlsx
@@ -5,23 +5,30 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Software Engineering\Assignment 1\Iteration4\After Coding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Software Engineering\Assignment 1\Iteration5\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6517F174-FC72-4906-87AD-CDDFC02A0BA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{6517F174-FC72-4906-87AD-CDDFC02A0BA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{2ECBC0B6-E071-4FDB-8079-E5323C8DEB1D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="94">
   <si>
     <t>PSP Defect Recording Log</t>
   </si>
@@ -668,6 +675,21 @@
   </si>
   <si>
     <t>[Vue warn]: Invalid prop: type check failed for prop "currentStatement". Expected String with value "82", got Number with value 82. - .toString() added</t>
+  </si>
+  <si>
+    <t>[Vue warn]: Error in data(): "TypeError: _model.GameOne is not a constructor" - Need to export class</t>
+  </si>
+  <si>
+    <t>[Vue warn]: Invalid prop: type check failed for prop "guess". Expected Number with value NaN, got String with value "Cheating?". - String check (typeof/instanceof String)</t>
+  </si>
+  <si>
+    <t>[Vue warn]: Error in v-on handler: "TypeError: Cannot read property 'toString' of undefined" - Extra else statement needed to return string</t>
+  </si>
+  <si>
+    <t>[Vue warn]: Error in render: "TypeError: Cannot read property 'toString' of undefined" - Needed super(newGuess, gameNumber)</t>
+  </si>
+  <si>
+    <t>Endless Loop. Crashed browser. When check if number had been used before, if all numbers had been used then it would crash the browser. - Added check to prevent this</t>
   </si>
 </sst>
 </file>
@@ -1326,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,20 +1936,140 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H31" s="6"/>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
+        <v>43586</v>
+      </c>
+      <c r="B27">
+        <v>21</v>
+      </c>
+      <c r="C27">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <f>B27</f>
+        <v>21</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="18">
+        <v>43586</v>
+      </c>
+      <c r="B28">
+        <v>22</v>
+      </c>
+      <c r="C28">
+        <v>60</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28:G31" si="0">B28</f>
+        <v>22</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="18">
+        <v>43586</v>
+      </c>
+      <c r="B29">
+        <v>23</v>
+      </c>
+      <c r="C29">
+        <v>80</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
+        <v>43586</v>
+      </c>
+      <c r="B30">
+        <v>24</v>
+      </c>
+      <c r="C30">
+        <v>70</v>
+      </c>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
+        <v>43586</v>
+      </c>
+      <c r="B31">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>60</v>
+      </c>
+      <c r="D31" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H32" s="6"/>
@@ -2009,6 +2151,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>